<commit_message>
Sun Feb  2 15:11:44 CET 2025
</commit_message>
<xml_diff>
--- a/_GPO/Progetto/Project Manager/Project Controller 5IB_n_X.xlsx
+++ b/_GPO/Progetto/Project Manager/Project Controller 5IB_n_X.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/origgi/Desktop/StefanoOriggi/_GPO/Progetto/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/origgi/Desktop/StefanoOriggi/_GPO/Progetto/Project Manager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56EAF4C-6043-8947-8E04-1EB1AD2A4D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031DB0E7-80F3-284C-A76E-50B1DAC99714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="860" windowWidth="32040" windowHeight="20860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="880" windowWidth="30320" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REPORT" sheetId="1" r:id="rId1"/>
-    <sheet name="DOCUMENTI (ROSSO)" sheetId="5" r:id="rId2"/>
-    <sheet name="DOCUMENTI (VERDE)" sheetId="6" r:id="rId3"/>
+    <sheet name="DOCUMENTI (VERDE)" sheetId="6" r:id="rId2"/>
+    <sheet name="DOCUMENTI (ROSSO)" sheetId="5" r:id="rId3"/>
     <sheet name="DOCUMENTI(BIANCO)" sheetId="3" r:id="rId4"/>
     <sheet name="EMAIL" sheetId="4" r:id="rId5"/>
     <sheet name="DATI" sheetId="2" state="hidden" r:id="rId6"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="94">
   <si>
     <t>Monitoraggio e Controllo Globale</t>
   </si>
@@ -145,33 +145,18 @@
     <t xml:space="preserve">FRANCESCHINI </t>
   </si>
   <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 1</t>
-  </si>
-  <si>
     <t>2° Componente</t>
   </si>
   <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 2</t>
-  </si>
-  <si>
     <t>3° Componente</t>
   </si>
   <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 3</t>
-  </si>
-  <si>
     <t>4° Componente</t>
   </si>
   <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 4</t>
-  </si>
-  <si>
     <t>5° Componente</t>
   </si>
   <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 5</t>
-  </si>
-  <si>
     <t>**************************************************  GRUPPO VERDE  **************************************************</t>
   </si>
   <si>
@@ -247,18 +232,6 @@
     <t>Il report finale</t>
   </si>
   <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 6</t>
-  </si>
-  <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 7</t>
-  </si>
-  <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 8</t>
-  </si>
-  <si>
-    <t>Inserire qui una breve descrizione del lavoro assegnato al componente 9</t>
-  </si>
-  <si>
     <t>6° Componente</t>
   </si>
   <si>
@@ -323,6 +296,33 @@
   </si>
   <si>
     <t>5IB</t>
+  </si>
+  <si>
+    <t>Business case</t>
+  </si>
+  <si>
+    <t>Organizzazione Settimana successiva</t>
+  </si>
+  <si>
+    <t>Project charter</t>
+  </si>
+  <si>
+    <t>Scope statement</t>
+  </si>
+  <si>
+    <t>Organizzazione team e settimana successiva</t>
+  </si>
+  <si>
+    <t>Ritardo</t>
+  </si>
+  <si>
+    <t>Organizzazione Settimana successiva, gantt</t>
+  </si>
+  <si>
+    <t>Organizzazione settimana successiva</t>
+  </si>
+  <si>
+    <t>Organizzazione team e settimana successiva; Gantt</t>
   </si>
 </sst>
 </file>
@@ -1533,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="125" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1551,7 +1551,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="13" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="26" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B1" s="66" t="s">
         <v>0</v>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="44" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B6" s="60"/>
       <c r="C6" s="16" t="s">
@@ -1682,19 +1682,19 @@
         <v>16</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G7" s="45" t="s">
         <v>16</v>
       </c>
       <c r="H7" s="44" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="I7" s="72"/>
       <c r="J7" s="73"/>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="I13" s="49"/>
       <c r="J13" s="48" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="K13" s="48"/>
     </row>
@@ -1840,161 +1840,211 @@
         <v>32</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="D15" s="46"/>
       <c r="E15" s="46"/>
       <c r="F15" s="46"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="47"/>
+      <c r="G15" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="21">
+        <v>5</v>
+      </c>
+      <c r="I15" s="21">
+        <v>7</v>
+      </c>
+      <c r="J15" s="47">
+        <v>1</v>
+      </c>
       <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:12" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="D16" s="46"/>
       <c r="E16" s="46"/>
       <c r="F16" s="46"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="47"/>
+      <c r="G16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="21">
+        <v>5</v>
+      </c>
+      <c r="I16" s="21">
+        <v>7</v>
+      </c>
+      <c r="J16" s="47">
+        <v>1</v>
+      </c>
       <c r="K16" s="47"/>
     </row>
     <row r="17" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D17" s="46"/>
       <c r="E17" s="46"/>
       <c r="F17" s="46"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="G17" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="21">
+        <v>5</v>
+      </c>
+      <c r="I17" s="21">
+        <v>7</v>
+      </c>
       <c r="J17" s="47"/>
       <c r="K17" s="47"/>
     </row>
     <row r="18" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="D18" s="46"/>
       <c r="E18" s="46"/>
       <c r="F18" s="46"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="G18" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="21">
+        <v>5</v>
+      </c>
+      <c r="I18" s="21">
+        <v>7</v>
+      </c>
       <c r="J18" s="47"/>
       <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="G19" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="21">
+        <v>5</v>
+      </c>
+      <c r="I19" s="21">
+        <v>7</v>
+      </c>
       <c r="J19" s="47"/>
       <c r="K19" s="47"/>
     </row>
     <row r="20" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D20" s="46"/>
       <c r="E20" s="46"/>
       <c r="F20" s="46"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="G20" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="21">
+        <v>5</v>
+      </c>
+      <c r="I20" s="21">
+        <v>7</v>
+      </c>
       <c r="J20" s="47"/>
       <c r="K20" s="47"/>
     </row>
     <row r="21" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
       <c r="D21" s="46"/>
       <c r="E21" s="46"/>
       <c r="F21" s="46"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="G21" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="21">
+        <v>5</v>
+      </c>
+      <c r="I21" s="21">
+        <v>7</v>
+      </c>
       <c r="J21" s="47"/>
       <c r="K21" s="47"/>
     </row>
     <row r="22" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C22" s="46" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D22" s="46"/>
       <c r="E22" s="46"/>
       <c r="F22" s="46"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="G22" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="21">
+        <v>5</v>
+      </c>
+      <c r="I22" s="21">
+        <v>7</v>
+      </c>
       <c r="J22" s="47"/>
       <c r="K22" s="47"/>
     </row>
     <row r="23" spans="1:11" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="46" t="s">
-        <v>71</v>
-      </c>
+      <c r="C23" s="46"/>
       <c r="D23" s="46"/>
       <c r="E23" s="46"/>
       <c r="F23" s="46"/>
@@ -2006,7 +2056,7 @@
     </row>
     <row r="24" spans="1:11" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B24" s="56"/>
       <c r="C24" s="56"/>
@@ -2040,7 +2090,7 @@
       </c>
       <c r="I25" s="49"/>
       <c r="J25" s="48" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="K25" s="48"/>
     </row>
@@ -2066,161 +2116,211 @@
         <v>32</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="D27" s="46"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="47"/>
+      <c r="G27" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="21">
+        <v>5</v>
+      </c>
+      <c r="I27" s="21">
+        <v>7</v>
+      </c>
+      <c r="J27" s="47">
+        <v>1</v>
+      </c>
       <c r="K27" s="47"/>
     </row>
     <row r="28" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="D28" s="46"/>
       <c r="E28" s="46"/>
       <c r="F28" s="46"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="G28" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="21">
+        <v>5</v>
+      </c>
+      <c r="I28" s="21">
+        <v>7</v>
+      </c>
       <c r="J28" s="47"/>
       <c r="K28" s="47"/>
     </row>
     <row r="29" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D29" s="46"/>
       <c r="E29" s="46"/>
       <c r="F29" s="46"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+      <c r="G29" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="21">
+        <v>5</v>
+      </c>
+      <c r="I29" s="21">
+        <v>7</v>
+      </c>
       <c r="J29" s="47"/>
       <c r="K29" s="47"/>
     </row>
     <row r="30" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="D30" s="46"/>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
+      <c r="G30" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="21">
+        <v>5</v>
+      </c>
+      <c r="I30" s="21">
+        <v>7</v>
+      </c>
       <c r="J30" s="47"/>
       <c r="K30" s="47"/>
     </row>
     <row r="31" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="D31" s="46"/>
       <c r="E31" s="46"/>
       <c r="F31" s="46"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
+      <c r="G31" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="21">
+        <v>5</v>
+      </c>
+      <c r="I31" s="21">
+        <v>7</v>
+      </c>
       <c r="J31" s="47"/>
       <c r="K31" s="47"/>
     </row>
     <row r="32" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D32" s="46"/>
       <c r="E32" s="46"/>
       <c r="F32" s="46"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
+      <c r="G32" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="21">
+        <v>5</v>
+      </c>
+      <c r="I32" s="21">
+        <v>7</v>
+      </c>
       <c r="J32" s="47"/>
       <c r="K32" s="47"/>
     </row>
     <row r="33" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D33" s="46"/>
       <c r="E33" s="46"/>
       <c r="F33" s="46"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="47"/>
+      <c r="G33" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="21">
+        <v>5</v>
+      </c>
+      <c r="I33" s="21">
+        <v>7</v>
+      </c>
+      <c r="J33" s="47">
+        <v>1</v>
+      </c>
       <c r="K33" s="47"/>
     </row>
     <row r="34" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D34" s="46"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
+      <c r="G34" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="21">
+        <v>5</v>
+      </c>
+      <c r="I34" s="21">
+        <v>7</v>
+      </c>
       <c r="J34" s="47"/>
       <c r="K34" s="47"/>
     </row>
     <row r="35" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="46" t="s">
-        <v>71</v>
-      </c>
+      <c r="C35" s="46"/>
       <c r="D35" s="46"/>
       <c r="E35" s="46"/>
       <c r="F35" s="46"/>
@@ -2232,7 +2332,7 @@
     </row>
     <row r="37" spans="1:11" ht="19.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="52" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B37" s="53"/>
       <c r="C37" s="53"/>
@@ -2266,7 +2366,7 @@
       </c>
       <c r="I38" s="49"/>
       <c r="J38" s="48" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="K38" s="48"/>
     </row>
@@ -2292,144 +2392,196 @@
         <v>32</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="D40" s="46"/>
       <c r="E40" s="46"/>
       <c r="F40" s="46"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="47"/>
+      <c r="G40" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="21">
+        <v>5</v>
+      </c>
+      <c r="I40" s="21">
+        <v>7</v>
+      </c>
+      <c r="J40" s="47">
+        <v>1</v>
+      </c>
       <c r="K40" s="47"/>
     </row>
     <row r="41" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="46" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="D41" s="46"/>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="47"/>
+      <c r="G41" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="21">
+        <v>6</v>
+      </c>
+      <c r="I41" s="21">
+        <v>8</v>
+      </c>
+      <c r="J41" s="47">
+        <v>0.4</v>
+      </c>
       <c r="K41" s="47"/>
     </row>
     <row r="42" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C42" s="46" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
       <c r="D42" s="46"/>
       <c r="E42" s="46"/>
       <c r="F42" s="46"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="47"/>
+      <c r="G42" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H42" s="21">
+        <v>6</v>
+      </c>
+      <c r="I42" s="21">
+        <v>8</v>
+      </c>
+      <c r="J42" s="47">
+        <v>0.4</v>
+      </c>
       <c r="K42" s="47"/>
     </row>
     <row r="43" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C43" s="46" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="D43" s="46"/>
       <c r="E43" s="46"/>
       <c r="F43" s="46"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="47"/>
+      <c r="G43" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H43" s="21">
+        <v>5</v>
+      </c>
+      <c r="I43" s="21">
+        <v>7</v>
+      </c>
+      <c r="J43" s="47">
+        <v>0.9</v>
+      </c>
       <c r="K43" s="47"/>
     </row>
     <row r="44" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C44" s="46" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D44" s="46"/>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="47"/>
+      <c r="G44" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="H44" s="21">
+        <v>5</v>
+      </c>
+      <c r="I44" s="21">
+        <v>7</v>
+      </c>
+      <c r="J44" s="47">
+        <v>0.9</v>
+      </c>
       <c r="K44" s="47"/>
     </row>
     <row r="45" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="46" t="s">
         <v>88</v>
-      </c>
-      <c r="C45" s="46" t="s">
-        <v>68</v>
       </c>
       <c r="D45" s="46"/>
       <c r="E45" s="46"/>
       <c r="F45" s="46"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="47"/>
+      <c r="G45" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="21">
+        <v>7</v>
+      </c>
+      <c r="I45" s="21">
+        <v>9</v>
+      </c>
+      <c r="J45" s="47">
+        <v>0.3</v>
+      </c>
       <c r="K45" s="47"/>
     </row>
     <row r="46" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C46" s="46" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D46" s="46"/>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="47"/>
+      <c r="G46" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="21">
+        <v>7</v>
+      </c>
+      <c r="I46" s="21">
+        <v>9</v>
+      </c>
+      <c r="J46" s="47">
+        <v>0.3</v>
+      </c>
       <c r="K46" s="47"/>
     </row>
     <row r="47" spans="1:11" ht="47" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C47" s="46" t="s">
-        <v>70</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="46"/>
       <c r="D47" s="46"/>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
@@ -2441,12 +2593,10 @@
     </row>
     <row r="48" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B48" s="3"/>
-      <c r="C48" s="46" t="s">
-        <v>71</v>
-      </c>
+      <c r="C48" s="46"/>
       <c r="D48" s="46"/>
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
@@ -2658,11 +2808,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8DB2FE-BA02-FD48-A48B-DF21F1E71450}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082A5F4E-4643-FF40-8E58-F99EF4A28EE6}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="108" zoomScaleNormal="100" zoomScalePageLayoutView="108" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView view="pageLayout" zoomScale="108" zoomScaleNormal="100" zoomScalePageLayoutView="108" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -2678,10 +2828,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2689,178 +2839,492 @@
         <v>1</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="39"/>
+        <v>43</v>
+      </c>
+      <c r="C2" s="39">
+        <v>45687</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="36">
         <v>2</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="39"/>
+        <v>44</v>
+      </c>
+      <c r="C3" s="39">
+        <v>45691</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="36">
         <v>3</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="39"/>
+        <v>45</v>
+      </c>
+      <c r="C4" s="39">
+        <v>45694</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="36">
         <v>4</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="39"/>
+        <v>46</v>
+      </c>
+      <c r="C5" s="39">
+        <v>45698</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="36">
         <v>5</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="39"/>
+        <v>47</v>
+      </c>
+      <c r="C6" s="39">
+        <v>45701</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="36">
         <v>6</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="39"/>
+        <v>48</v>
+      </c>
+      <c r="C7" s="39">
+        <v>45705</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="36">
         <v>7</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="39"/>
+        <v>49</v>
+      </c>
+      <c r="C8" s="39">
+        <v>45708</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
         <v>8</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="39"/>
+        <v>50</v>
+      </c>
+      <c r="C9" s="39">
+        <v>45712</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <v>9</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="39"/>
+        <v>51</v>
+      </c>
+      <c r="C10" s="39">
+        <v>45715</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
         <v>10</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="39"/>
+        <v>52</v>
+      </c>
+      <c r="C11" s="39">
+        <v>45719</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="36">
         <v>11</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="39"/>
+        <v>53</v>
+      </c>
+      <c r="C12" s="39">
+        <v>45722</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="36">
         <v>12</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="39"/>
+        <v>54</v>
+      </c>
+      <c r="C13" s="39">
+        <v>45729</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="36">
         <v>13</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="39"/>
+        <v>55</v>
+      </c>
+      <c r="C14" s="39">
+        <v>45733</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="36">
         <v>14</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="39"/>
+        <v>56</v>
+      </c>
+      <c r="C15" s="39">
+        <v>45736</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="36">
         <v>15</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="39"/>
+        <v>57</v>
+      </c>
+      <c r="C16" s="39">
+        <v>45740</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="36">
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="39"/>
+        <v>58</v>
+      </c>
+      <c r="C17" s="39">
+        <v>45750</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="36">
         <v>17</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="39"/>
+        <v>59</v>
+      </c>
+      <c r="C18" s="39">
+        <v>45754</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="36">
         <v>18</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="39"/>
+        <v>60</v>
+      </c>
+      <c r="C19" s="39">
+        <v>45757</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="36">
         <v>19</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="39"/>
+        <v>61</v>
+      </c>
+      <c r="C20" s="39">
+        <v>45761</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36">
         <v>20</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+      <c r="C21" s="39">
+        <v>45775</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.humanwareonline.com/project-management/center/business-case/" xr:uid="{4059450D-3D9B-B74F-95B2-68B436A8A9FD}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.humanwareonline.com/project-management/center/avviare-un-progetto/" xr:uid="{5E87D973-3320-2340-BDC5-1B128B5B2C2F}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.humanwareonline.com/project-management/center/scope-statement/" xr:uid="{FDC56985-DC92-D543-AD94-73692DAD82DD}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://www.humanwareonline.com/project-management/center/wbs-work-breakdown-structure/" xr:uid="{68803125-9663-DB44-85F9-C87EDEB60959}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://www.humanwareonline.com/project-management/center/obs-progetto-struttura-organigramma/" xr:uid="{D7810F7B-D671-3A4A-A85F-12056F6569B3}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://www.humanwareonline.com/project-management/center/ram-matrice-assegnazione-responsabilita/" xr:uid="{65F7BE87-BEFE-A049-8EDE-69FA809F4003}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://www.humanwareonline.com/project-management/center/gantt-di-progetto/" xr:uid="{DFB40893-CA65-5347-ACA7-0F75BB95B1E7}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://www.humanwareonline.com/project-management/center/costi-budget-progetto/" xr:uid="{E31B756B-924C-5043-805B-AD7AE6F34DE2}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://www.humanwareonline.com/project-management/center/stima-risorse-di-progetto/" xr:uid="{45A3106A-9C1C-8945-AD4F-788AB27F27C0}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.humanwareonline.com/project-management/center/piano-qualita-progetto/" xr:uid="{77FF30D4-23F9-0146-8768-BEEE90EF885C}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.humanwareonline.com/project-management/center/gestione-rischi-progetto/" xr:uid="{2F9C7B6F-0ECF-3A4D-9DB2-79220B7CE286}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.humanwareonline.com/project-management/center/comunicazione-di-progetto/" xr:uid="{ED87A9A5-5B4A-3F4A-B2CC-405C8DAD8EAD}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.humanwareonline.com/project-management/center/project-procurement-contratti/" xr:uid="{8A7ADC44-86FD-8343-94C5-B88DB51640CA}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.humanwareonline.com/project-management/center/piano-di-progetto/" xr:uid="{A191CA05-6BBF-264A-9E70-E50CD3CAF932}"/>
+    <hyperlink ref="B18" r:id="rId15" display="https://www.humanwareonline.com/project-management/center/project-status-report/" xr:uid="{D13949F6-F215-E848-814F-39C7B2B0DFCD}"/>
+    <hyperlink ref="B20" r:id="rId16" display="https://www.humanwareonline.com/project-management/center/controllo-progetto-monitoraggio-avanzamento/" xr:uid="{5E21B95F-4E55-D64F-9D18-A81B1CCFE34E}"/>
+    <hyperlink ref="B21" r:id="rId17" display="https://www.humanwareonline.com/project-management/center/chiusura-progetto-report-lesson-learned/" xr:uid="{68A349B5-DC55-DE42-9612-B8C3ED361BC6}"/>
+  </hyperlinks>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"-,Grassetto"&amp;20MAPPA DEI DOCUMENTI DA PRODURRE</oddHeader>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FC67E4D-38B9-2C40-88EC-EE4D0186D864}">
+          <x14:formula1>
+            <xm:f>DATI!$D$1:$D$96</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8DB2FE-BA02-FD48-A48B-DF21F1E71450}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScale="108" zoomScaleNormal="100" zoomScalePageLayoutView="108" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="76.5" style="32" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="32" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="39">
+        <v>45690</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36">
+        <v>2</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="39">
+        <v>45696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36">
+        <v>3</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="39">
+        <v>45703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36">
+        <v>4</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="39">
+        <v>45710</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36">
+        <v>5</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="39">
+        <v>45717</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36">
+        <v>6</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="39">
+        <v>45724</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="36">
+        <v>7</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="39">
+        <v>45731</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36">
+        <v>8</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="39">
+        <v>45738</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="36">
+        <v>9</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="39">
+        <v>45745</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="36">
+        <v>10</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="39">
+        <v>45752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="36">
+        <v>11</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="39">
+        <v>45759</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="36">
+        <v>12</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="39">
+        <v>45766</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="36">
+        <v>13</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="39">
+        <v>45773</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="36">
+        <v>14</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="39"/>
+    </row>
+    <row r="16" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="36">
+        <v>15</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="39"/>
+    </row>
+    <row r="17" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="36">
+        <v>16</v>
+      </c>
+      <c r="B17" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="39"/>
+    </row>
+    <row r="18" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="36">
+        <v>17</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="39"/>
+    </row>
+    <row r="19" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="36">
+        <v>18</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="39"/>
+    </row>
+    <row r="20" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36">
+        <v>19</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="39"/>
+    </row>
+    <row r="21" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36">
+        <v>20</v>
+      </c>
+      <c r="B21" s="37" t="s">
+        <v>62</v>
       </c>
       <c r="C21" s="39"/>
     </row>
@@ -2905,12 +3369,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082A5F4E-4643-FF40-8E58-F99EF4A28EE6}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6A75C3-8E97-4030-8C23-61187FC28C3F}">
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="108" zoomScaleNormal="100" zoomScalePageLayoutView="108" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
@@ -2926,10 +3390,10 @@
         <v>1</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2937,7 +3401,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C2" s="39"/>
     </row>
@@ -2946,7 +3410,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" s="39"/>
     </row>
@@ -2955,7 +3419,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C4" s="39"/>
     </row>
@@ -2964,7 +3428,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" s="39"/>
     </row>
@@ -2973,7 +3437,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C6" s="39"/>
     </row>
@@ -2982,7 +3446,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C7" s="39"/>
     </row>
@@ -2991,7 +3455,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C8" s="39"/>
     </row>
@@ -3000,7 +3464,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9" s="39"/>
     </row>
@@ -3009,7 +3473,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C10" s="39"/>
     </row>
@@ -3018,7 +3482,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C11" s="39"/>
     </row>
@@ -3027,7 +3491,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C12" s="39"/>
     </row>
@@ -3036,7 +3500,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C13" s="39"/>
     </row>
@@ -3045,7 +3509,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C14" s="39"/>
     </row>
@@ -3054,7 +3518,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C15" s="39"/>
     </row>
@@ -3063,7 +3527,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C16" s="39"/>
     </row>
@@ -3072,7 +3536,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C17" s="39"/>
     </row>
@@ -3081,7 +3545,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C18" s="39"/>
     </row>
@@ -3090,7 +3554,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="38" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C19" s="39"/>
     </row>
@@ -3099,7 +3563,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C20" s="39"/>
     </row>
@@ -3108,255 +3572,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="39"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.humanwareonline.com/project-management/center/business-case/" xr:uid="{4059450D-3D9B-B74F-95B2-68B436A8A9FD}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://www.humanwareonline.com/project-management/center/avviare-un-progetto/" xr:uid="{5E87D973-3320-2340-BDC5-1B128B5B2C2F}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://www.humanwareonline.com/project-management/center/scope-statement/" xr:uid="{FDC56985-DC92-D543-AD94-73692DAD82DD}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://www.humanwareonline.com/project-management/center/wbs-work-breakdown-structure/" xr:uid="{68803125-9663-DB44-85F9-C87EDEB60959}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://www.humanwareonline.com/project-management/center/obs-progetto-struttura-organigramma/" xr:uid="{D7810F7B-D671-3A4A-A85F-12056F6569B3}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://www.humanwareonline.com/project-management/center/ram-matrice-assegnazione-responsabilita/" xr:uid="{65F7BE87-BEFE-A049-8EDE-69FA809F4003}"/>
-    <hyperlink ref="B8" r:id="rId7" display="https://www.humanwareonline.com/project-management/center/gantt-di-progetto/" xr:uid="{DFB40893-CA65-5347-ACA7-0F75BB95B1E7}"/>
-    <hyperlink ref="B9" r:id="rId8" display="https://www.humanwareonline.com/project-management/center/costi-budget-progetto/" xr:uid="{E31B756B-924C-5043-805B-AD7AE6F34DE2}"/>
-    <hyperlink ref="B10" r:id="rId9" display="https://www.humanwareonline.com/project-management/center/stima-risorse-di-progetto/" xr:uid="{45A3106A-9C1C-8945-AD4F-788AB27F27C0}"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.humanwareonline.com/project-management/center/piano-qualita-progetto/" xr:uid="{77FF30D4-23F9-0146-8768-BEEE90EF885C}"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.humanwareonline.com/project-management/center/gestione-rischi-progetto/" xr:uid="{2F9C7B6F-0ECF-3A4D-9DB2-79220B7CE286}"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.humanwareonline.com/project-management/center/comunicazione-di-progetto/" xr:uid="{ED87A9A5-5B4A-3F4A-B2CC-405C8DAD8EAD}"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.humanwareonline.com/project-management/center/project-procurement-contratti/" xr:uid="{8A7ADC44-86FD-8343-94C5-B88DB51640CA}"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.humanwareonline.com/project-management/center/piano-di-progetto/" xr:uid="{A191CA05-6BBF-264A-9E70-E50CD3CAF932}"/>
-    <hyperlink ref="B18" r:id="rId15" display="https://www.humanwareonline.com/project-management/center/project-status-report/" xr:uid="{D13949F6-F215-E848-814F-39C7B2B0DFCD}"/>
-    <hyperlink ref="B20" r:id="rId16" display="https://www.humanwareonline.com/project-management/center/controllo-progetto-monitoraggio-avanzamento/" xr:uid="{5E21B95F-4E55-D64F-9D18-A81B1CCFE34E}"/>
-    <hyperlink ref="B21" r:id="rId17" display="https://www.humanwareonline.com/project-management/center/chiusura-progetto-report-lesson-learned/" xr:uid="{68A349B5-DC55-DE42-9612-B8C3ED361BC6}"/>
-  </hyperlinks>
-  <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"-,Grassetto"&amp;20MAPPA DEI DOCUMENTI DA PRODURRE</oddHeader>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5C850997-1034-7648-96A8-7E1DE350A471}">
-          <x14:formula1>
-            <xm:f>DATI!$D$1:$D$96</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C21</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6A75C3-8E97-4030-8C23-61187FC28C3F}">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView view="pageLayout" zoomScale="108" zoomScaleNormal="100" zoomScalePageLayoutView="108" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="17" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="5.33203125" style="33" customWidth="1"/>
-    <col min="2" max="2" width="76.5" style="32" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="32" customWidth="1"/>
-    <col min="4" max="16384" width="9.1640625" style="32"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36">
-        <v>1</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="39"/>
-    </row>
-    <row r="3" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36">
-        <v>2</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="39"/>
-    </row>
-    <row r="4" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36">
-        <v>3</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="39"/>
-    </row>
-    <row r="5" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36">
-        <v>4</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="39"/>
-    </row>
-    <row r="6" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="36">
-        <v>5</v>
-      </c>
-      <c r="B6" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="39"/>
-    </row>
-    <row r="7" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="36">
-        <v>6</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="39"/>
-    </row>
-    <row r="8" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="36">
-        <v>7</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="39"/>
-    </row>
-    <row r="9" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="36">
-        <v>8</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="39"/>
-    </row>
-    <row r="10" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="36">
-        <v>9</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="39"/>
-    </row>
-    <row r="11" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="36">
-        <v>10</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="39"/>
-    </row>
-    <row r="12" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="36">
-        <v>11</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="39"/>
-    </row>
-    <row r="13" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="36">
-        <v>12</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="39"/>
-    </row>
-    <row r="14" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="36">
-        <v>13</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="39"/>
-    </row>
-    <row r="15" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="36">
-        <v>14</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="39"/>
-    </row>
-    <row r="16" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="36">
-        <v>15</v>
-      </c>
-      <c r="B16" s="37" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" s="39"/>
-    </row>
-    <row r="17" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="36">
-        <v>16</v>
-      </c>
-      <c r="B17" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="39"/>
-    </row>
-    <row r="18" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="36">
-        <v>17</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="39"/>
-    </row>
-    <row r="19" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="36">
-        <v>18</v>
-      </c>
-      <c r="B19" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="C19" s="39"/>
-    </row>
-    <row r="20" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="36">
-        <v>19</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="39"/>
-    </row>
-    <row r="21" spans="1:3" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="36">
-        <v>20</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>67</v>
       </c>
       <c r="C21" s="39"/>
     </row>
@@ -3388,7 +3604,7 @@
   </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB899504-3418-487D-BC5B-6915DF9B8374}">
           <x14:formula1>
             <xm:f>DATI!$D$1:$D$96</xm:f>
@@ -3406,7 +3622,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="169" zoomScaleNormal="100" zoomScalePageLayoutView="169" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3508,7 +3724,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="43" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D1" s="31">
         <v>45682</v>
@@ -3525,7 +3741,7 @@
         <v>0.1</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D2" s="31">
         <v>45683</v>
@@ -3539,7 +3755,7 @@
         <v>0.2</v>
       </c>
       <c r="C3" s="43" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D3" s="31">
         <v>45684</v>
@@ -3553,7 +3769,7 @@
         <v>0.3</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D4" s="31">
         <v>45685</v>
@@ -3567,7 +3783,7 @@
         <v>0.4</v>
       </c>
       <c r="C5" s="43" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="D5" s="31">
         <v>45686</v>
@@ -3595,7 +3811,7 @@
         <v>0.6</v>
       </c>
       <c r="C7" s="43" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D7" s="31">
         <v>45688</v>
@@ -3637,7 +3853,7 @@
         <v>0.9</v>
       </c>
       <c r="C10" s="43" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D10" s="31">
         <v>45691</v>
@@ -3651,7 +3867,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="43" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D11" s="31">
         <v>45692</v>
@@ -3693,7 +3909,7 @@
         <v>1.3</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D14" s="31">
         <v>45695</v>
@@ -3707,7 +3923,7 @@
         <v>1.4</v>
       </c>
       <c r="C15" s="43" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D15" s="31">
         <v>45696</v>
@@ -3721,7 +3937,7 @@
         <v>1.5</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D16" s="31">
         <v>45697</v>
@@ -3735,7 +3951,7 @@
         <v>1.6</v>
       </c>
       <c r="C17" s="43" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D17" s="31">
         <v>45698</v>
@@ -3749,7 +3965,7 @@
         <v>1.7</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D18" s="31">
         <v>45699</v>
@@ -3763,7 +3979,7 @@
         <v>1.8</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D19" s="31">
         <v>45700</v>
@@ -3777,7 +3993,7 @@
         <v>1.9</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D20" s="31">
         <v>45701</v>
@@ -3791,7 +4007,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D21" s="31">
         <v>45702</v>
@@ -3805,7 +4021,7 @@
         <v>2.1</v>
       </c>
       <c r="C22" s="43" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D22" s="31">
         <v>45703</v>
@@ -3819,7 +4035,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D23" s="31">
         <v>45704</v>
@@ -3833,7 +4049,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C24" s="43" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D24" s="31">
         <v>45705</v>

</xml_diff>